<commit_message>
feat: typhoon xlsx 更新说明文档
Signed-off-by: stanleyguo0207 <stanleyguo0207@163.com>
</commit_message>
<xml_diff>
--- a/tpn/tools/xlsx2data/demo/dungeon.xlsx
+++ b/tpn/tools/xlsx2data/demo/dungeon.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="936" yWindow="0" windowWidth="22260" windowHeight="12648"/>
+    <workbookView xWindow="1872" yWindow="0" windowWidth="22260" windowHeight="12648"/>
   </bookViews>
   <sheets>
     <sheet name="@DungeonA" sheetId="1" r:id="rId1"/>
@@ -20,31 +20,16 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
-  <si>
-    <t>id[u16][!]</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>副本id</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>name[str][*]</t>
-  </si>
-  <si>
     <t>副本名称</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>1001,100|1002,300</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>awards[u32,u32][*][Item.id,|]</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>关卡1</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -69,23 +54,37 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>1001,100|1002,400</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>1001,100|1002,500</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>1001,100|1002,600</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>1001,100|1002,700</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>1001,100|1002,800</t>
+    <t>副本掉落</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>id[u16][!][]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>name[str][*][C]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1001-100|1002-300</t>
+  </si>
+  <si>
+    <t>1001-100|1002-400</t>
+  </si>
+  <si>
+    <t>1001-100|1002-500</t>
+  </si>
+  <si>
+    <t>1001-100|1002-600</t>
+  </si>
+  <si>
+    <t>1001-100|1002-700</t>
+  </si>
+  <si>
+    <t>1001-100|1002-800</t>
+  </si>
+  <si>
+    <t>awards[u16-u32|][*][][Item.id-$|]</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -414,36 +413,36 @@
   <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="26.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="31.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="B1" t="s">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="C1" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
-        <v>3</v>
-      </c>
       <c r="C2" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -451,10 +450,10 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -462,7 +461,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="C4" t="s">
         <v>12</v>
@@ -473,7 +472,7 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C5" t="s">
         <v>13</v>
@@ -484,7 +483,7 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C6" t="s">
         <v>14</v>
@@ -495,7 +494,7 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C7" t="s">
         <v>15</v>
@@ -506,7 +505,7 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C8" t="s">
         <v>16</v>
@@ -515,6 +514,7 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>